<commit_message>
need a fresh commmit for gitcli token regen
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1695" count="1695">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92" count="92">
   <x:si>
     <x:t>message</x:t>
   </x:si>
@@ -28,88 +28,268 @@
     <x:t>datum</x:t>
   </x:si>
   <x:si>
-    <x:t>lighthouse check initiated at Tue Aug 24 2021 14:52:28 GMT-0600 (Mountain Daylight Time)</x:t>
+    <x:t>lighthouse check initiated at Fri Aug 27 2021 15:19:56 GMT-0600 (Mountain Daylight Time)</x:t>
   </x:si>
   <x:si>
     <x:t>n/a</x:t>
   </x:si>
   <x:si>
-    <x:t>https://tilecleaningorangecounty.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>best practices score</x:t>
-  </x:si>
-  <x:si>
-    <x:t>accessibility score</x:t>
-  </x:si>
-  <x:si>
-    <x:t>seo score</x:t>
+    <x:t/>
+  </x:si>
+  <x:si>
+    <x:t>https://asafs-locksmith.com</x:t>
   </x:si>
   <x:si>
     <x:t>mobile speed</x:t>
   </x:si>
   <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
     <x:t>desktop speed</x:t>
   </x:si>
   <x:si>
-    <x:t>https://westkyroofing.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://brevardtilecleaning.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://meangreencarpetcleaners.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ripleyservices.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://true-clean.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.absolutecarpetcarestl.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.cleanforceone.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://akrosteam.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://havencr.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://aladdincarpetcleaningsj.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://reddingcarpetcleaner.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.duracleanm.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.cleanhomepowerwashing.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://yourtrueclean.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://fusioncleaningcolorado.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://alamosteamteam.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://foothillsexterior.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://trojancarpetcare.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Lighthouse check completed at Tue Aug 24 2021 15:02:40 GMT-0600 (Mountain Daylight Time)</x:t>
+    <x:t>https://gatorcleaningbrevard.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://diamondcarpetcare.net/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://tilecleaningorangecounty.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://seethroughwindowcleaningatx.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://wizardcarpetcare.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bowenservicesllc.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://thatsawrapshrinkwrapping.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.xtremecleanaz.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://westkyroofing.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://mcaelectric.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://xtremecarpets.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.carpetmdinfo.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cleaningrestorationpros.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://staycleanli.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://brevardtilecleaning.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.choosewindowmagic.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cleanamericacarpetcleaning.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://meangreencarpetcleaners.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://dollbrothers.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://patriotpressurewashing.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://adenpressurewashing.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://ejpressurewashing.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://wewashproperties.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ripleyservices.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://signaturespb.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://true-clean.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://crystalsteem.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://asapcarpetcleaningbend.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://powercleanidaho.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://modernmechhvac.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://patriotairnd.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.acsfoothills.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://pcsraleigh.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://citruscleantampa.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://bardplumbing.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://freedompowerwashingllc.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.absolutecarpetcarestl.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://abshercarpetcare.net/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.cleanforceone.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://khssteamer.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>http://mecomasterelectricco.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://powercleansc.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://manhattanbeachcarpetcleaners.net/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://akrosteam.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://havencr.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://northtexassoftwash.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.one-call-services.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.naturalcleaningsystems.ca/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://mbheatingandair.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://aladdincarpetcleaningsj.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://absolutecarpetandfloors.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://chiefrestorationswmo.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://coolingpros.ky/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://unitedcarpetcare.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://minutedrycarpetcleaning.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://homebridgecanada.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.topshotpressurewash.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://reddingcarpetcleaner.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://allbritetx.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.duracleanm.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://lumenselectric.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.pmwpowerwash.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.cleanhomepowerwashing.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://yourtrueclean.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://eliteexteriorsolutionsmn.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://russspraguecarpetcleaning.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://fusioncleaningcolorado.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://alamosteamteam.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://repelecarpet.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://sanibrightcarpetcleaning.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://rgdecor.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://orientalrugcleaningindianapolis.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cleantimesoftwash.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://abelectricpro.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cleanitup843.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://champspowerwashing.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.carpetdrycleaners.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfortonthecoast.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.aeacleaningservices.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://foothillsexterior.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://trojancarpetcare.com/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lighthouse check completed at Fri Aug 27 2021 15:50:28 GMT-0600 (Mountain Daylight Time)</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -501,1119 +681,2313 @@
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
+      <x:c r="A3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="n">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="A4" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="n">
-        <x:v>93</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:4">
-      <x:c r="B4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D4" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
+      <x:c r="A5" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D5" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
+      <x:c r="A6" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D6" s="0" t="n">
-        <x:v>55.00000000000001</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
       <x:c r="A7" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
       <x:c r="C7" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="n">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:4">
+      <x:c r="A8" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="n">
+        <x:v>54</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="A9" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="n">
-        <x:v>59</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:4">
-      <x:c r="B8" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="n">
-        <x:v>93</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:4">
-      <x:c r="B9" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
       <x:c r="C9" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="D9" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>56.99999999999999</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
+      <x:c r="A10" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="D10" s="0" t="n">
-        <x:v>77</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
+      <x:c r="A11" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B11" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D11" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="A12" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D12" s="0" t="n">
-        <x:v>25</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
+      <x:c r="A13" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B13" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D13" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
+      <x:c r="A14" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B14" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D14" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
+      <x:c r="A15" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D15" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
+      <x:c r="A16" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D16" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
       <x:c r="A17" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D17" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
+      <x:c r="A18" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D18" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
+      <x:c r="A19" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="D19" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
+      <x:c r="A20" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="D20" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4">
+      <x:c r="A21" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D21" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:4">
       <x:c r="A22" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D22" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4">
+      <x:c r="A23" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D23" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:4">
+      <x:c r="A24" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D24" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:4">
+      <x:c r="A25" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D25" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:4">
+      <x:c r="A26" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D26" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:4">
       <x:c r="A27" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D27" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:4">
+      <x:c r="A28" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D28" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>55.00000000000001</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:4">
+      <x:c r="A29" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="D29" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:4">
+      <x:c r="A30" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="D30" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:4">
+      <x:c r="A31" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D31" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:4">
       <x:c r="A32" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C32" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D32" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:4">
+      <x:c r="A33" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D33" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:4">
+      <x:c r="A34" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D34" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:4">
+      <x:c r="A35" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D35" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:4">
+      <x:c r="A36" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C36" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D36" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:4">
       <x:c r="A37" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C37" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D37" s="0" t="n">
-        <x:v>33</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:4">
+      <x:c r="A38" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D38" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:4">
+      <x:c r="A39" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C39" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="D39" s="0" t="n">
-        <x:v>96</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:4">
+      <x:c r="A40" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C40" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="D40" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:4">
+      <x:c r="A41" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C41" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D41" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:4">
       <x:c r="A42" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C42" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D42" s="0" t="n">
-        <x:v>38</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:4">
+      <x:c r="A43" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C43" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D43" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>57.99999999999999</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:4">
+      <x:c r="A44" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C44" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D44" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:4">
+      <x:c r="A45" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C45" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D45" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:4">
+      <x:c r="A46" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C46" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D46" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:4">
       <x:c r="A47" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C47" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D47" s="0" t="n">
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:4">
+      <x:c r="A48" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D48" s="0" t="n">
         <x:v>38</x:v>
       </x:c>
     </x:row>
-    <x:row r="48" spans="1:4">
-      <x:c r="B48" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="C48" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D48" s="0" t="n">
-        <x:v>87</x:v>
-      </x:c>
-    </x:row>
     <x:row r="49" spans="1:4">
+      <x:c r="A49" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C49" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="D49" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:4">
+      <x:c r="A50" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C50" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="D50" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:4">
+      <x:c r="A51" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C51" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D51" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:4">
       <x:c r="A52" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C52" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D52" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:4">
+      <x:c r="A53" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C53" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D53" s="0" t="n">
+        <x:v>80</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:4">
+      <x:c r="A54" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C54" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D54" s="0" t="n">
+        <x:v>81</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:4">
+      <x:c r="A55" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C55" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D55" s="0" t="n">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D52" s="0" t="n">
-        <x:v>28.000000000000004</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="53" spans="1:4">
-      <x:c r="B53" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C53" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D53" s="0" t="n">
-        <x:v>93</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="54" spans="1:4">
-      <x:c r="B54" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C54" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D54" s="0" t="n">
-        <x:v>92</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="55" spans="1:4">
-      <x:c r="B55" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C55" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D55" s="0" t="n">
-        <x:v>75</x:v>
-      </x:c>
     </x:row>
     <x:row r="56" spans="1:4">
+      <x:c r="A56" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C56" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D56" s="0" t="n">
-        <x:v>44</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:4">
       <x:c r="A57" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C57" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D57" s="0" t="n">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:4">
+      <x:c r="A58" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C58" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D58" s="0" t="n">
+        <x:v>84</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:4">
+      <x:c r="A59" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-    </x:row>
-    <x:row r="58" spans="1:4">
-      <x:c r="B58" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C58" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D58" s="0" t="n">
+      <x:c r="C59" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D59" s="0" t="n">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:4">
+      <x:c r="A60" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C60" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D60" s="0" t="n">
         <x:v>73</x:v>
       </x:c>
     </x:row>
-    <x:row r="59" spans="1:4">
-      <x:c r="B59" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C59" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D59" s="0" t="n">
-        <x:v>83</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="60" spans="1:4">
-      <x:c r="B60" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C60" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="D60" s="0" t="n">
-        <x:v>68</x:v>
-      </x:c>
-    </x:row>
     <x:row r="61" spans="1:4">
+      <x:c r="A61" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C61" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D61" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:4">
       <x:c r="A62" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C62" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D62" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:4">
+      <x:c r="A63" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C63" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D63" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:4">
+      <x:c r="A64" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C64" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D64" s="0" t="n">
-        <x:v>85</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:4">
+      <x:c r="A65" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C65" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D65" s="0" t="n">
-        <x:v>67</x:v>
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:4">
+      <x:c r="A66" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B66" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C66" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D66" s="0" t="n">
-        <x:v>32</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:4">
       <x:c r="A67" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B67" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C67" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D67" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="68" spans="1:4">
+      <x:c r="A68" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B68" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C68" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D68" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="69" spans="1:4">
+      <x:c r="A69" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B69" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C69" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="D69" s="0" t="n">
-        <x:v>83</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="70" spans="1:4">
+      <x:c r="A70" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B70" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C70" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="D70" s="0" t="n">
-        <x:v>75</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="71" spans="1:4">
+      <x:c r="A71" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B71" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C71" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D71" s="0" t="n">
-        <x:v>40</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="72" spans="1:4">
       <x:c r="A72" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C72" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D72" s="0" t="n">
-        <x:v>43</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:4">
+      <x:c r="A73" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B73" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C73" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D73" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="74" spans="1:4">
+      <x:c r="A74" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B74" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C74" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D74" s="0" t="n">
-        <x:v>79</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:4">
+      <x:c r="A75" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B75" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C75" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D75" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:4">
+      <x:c r="A76" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B76" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C76" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D76" s="0" t="n">
-        <x:v>28.000000000000004</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="77" spans="1:4">
       <x:c r="A77" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B77" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C77" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D77" s="0" t="n">
-        <x:v>28.999999999999996</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:4">
+      <x:c r="A78" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B78" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C78" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D78" s="0" t="n">
-        <x:v>80</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:4">
+      <x:c r="A79" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B79" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C79" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="D79" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="80" spans="1:4">
+      <x:c r="A80" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B80" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C80" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="D80" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:4">
+      <x:c r="A81" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B81" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C81" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D81" s="0" t="n">
-        <x:v>15</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:4">
       <x:c r="A82" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B82" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C82" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D82" s="0" t="n">
-        <x:v>16</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:4">
+      <x:c r="A83" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B83" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C83" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D83" s="0" t="n">
-        <x:v>87</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:4">
+      <x:c r="A84" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B84" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C84" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D84" s="0" t="n">
-        <x:v>89</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:4">
+      <x:c r="A85" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B85" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C85" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D85" s="0" t="n">
-        <x:v>76</x:v>
+        <x:v>55.00000000000001</x:v>
       </x:c>
     </x:row>
     <x:row r="86" spans="1:4">
+      <x:c r="A86" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B86" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C86" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D86" s="0" t="n">
-        <x:v>7.000000000000001</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="87" spans="1:4">
       <x:c r="A87" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B87" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C87" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D87" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="1:4">
+      <x:c r="A88" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B88" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C88" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D88" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="89" spans="1:4">
+      <x:c r="A89" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B89" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C89" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="D89" s="0" t="n">
-        <x:v>88</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="90" spans="1:4">
+      <x:c r="A90" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B90" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C90" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="D90" s="0" t="n">
-        <x:v>71</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="91" spans="1:4">
+      <x:c r="A91" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B91" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C91" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D91" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="92" spans="1:4">
       <x:c r="A92" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B92" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C92" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D92" s="0" t="n">
-        <x:v>21</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="93" spans="1:4">
+      <x:c r="A93" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B93" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C93" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D93" s="0" t="n">
-        <x:v>93</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="94" spans="1:4">
+      <x:c r="A94" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B94" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C94" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D94" s="0" t="n">
-        <x:v>95</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="95" spans="1:4">
+      <x:c r="A95" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B95" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C95" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D95" s="0" t="n">
-        <x:v>86</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="96" spans="1:4">
+      <x:c r="A96" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
       <x:c r="B96" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C96" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D96" s="0" t="n">
-        <x:v>56.00000000000001</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="97" spans="1:4">
       <x:c r="A97" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B97" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C97" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D97" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>57.99999999999999</x:v>
       </x:c>
     </x:row>
     <x:row r="98" spans="1:4">
       <x:c r="A98" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B98" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C98" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D98" s="0" t="n">
+        <x:v>77</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:4">
+      <x:c r="A99" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C99" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D99" s="0" t="n">
+        <x:v>88</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:4">
+      <x:c r="A100" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C100" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D100" s="0" t="n">
+        <x:v>88</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" spans="1:4">
+      <x:c r="A101" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="C101" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D101" s="0" t="n">
+        <x:v>55.00000000000001</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" spans="1:4">
+      <x:c r="A102" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B102" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="C102" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D102" s="0" t="n">
+        <x:v>69</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103" spans="1:4">
+      <x:c r="A103" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B103" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="C103" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D103" s="0" t="n">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104" spans="1:4">
+      <x:c r="A104" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B104" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="C104" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D104" s="0" t="n">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="105" spans="1:4">
+      <x:c r="A105" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B105" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C105" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D105" s="0" t="n">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="106" spans="1:4">
+      <x:c r="A106" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B106" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C106" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D106" s="0" t="n">
+        <x:v>77</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="107" spans="1:4">
+      <x:c r="A107" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B107" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C107" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D107" s="0" t="n">
+        <x:v>77</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="108" spans="1:4">
+      <x:c r="A108" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B108" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C108" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D108" s="0" t="n">
+        <x:v>80</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="109" spans="1:4">
+      <x:c r="A109" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B109" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C109" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D109" s="0" t="n">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="110" spans="1:4">
+      <x:c r="A110" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B110" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C110" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D110" s="0" t="n">
+        <x:v>61</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="111" spans="1:4">
+      <x:c r="A111" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B111" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="C111" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D111" s="0" t="n">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="112" spans="1:4">
+      <x:c r="A112" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B112" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="C112" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D112" s="0" t="n">
+        <x:v>83</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="113" spans="1:4">
+      <x:c r="A113" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B113" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C113" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D113" s="0" t="n">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="114" spans="1:4">
+      <x:c r="A114" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B114" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C114" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D114" s="0" t="n">
+        <x:v>77</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="115" spans="1:4">
+      <x:c r="A115" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B115" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="C115" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D115" s="0" t="n">
+        <x:v>71</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="116" spans="1:4">
+      <x:c r="A116" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B116" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="C116" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D116" s="0" t="n">
+        <x:v>54</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="117" spans="1:4">
+      <x:c r="A117" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B117" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="C117" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D117" s="0" t="n">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="118" spans="1:4">
+      <x:c r="A118" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B118" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="C118" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D118" s="0" t="n">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="119" spans="1:4">
+      <x:c r="A119" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B119" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C119" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D119" s="0" t="n">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="120" spans="1:4">
+      <x:c r="A120" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B120" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C120" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D120" s="0" t="n">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="121" spans="1:4">
+      <x:c r="A121" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B121" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C121" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D121" s="0" t="n">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="122" spans="1:4">
+      <x:c r="A122" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B122" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C122" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D122" s="0" t="n">
+        <x:v>52</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="123" spans="1:4">
+      <x:c r="A123" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B123" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C123" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D123" s="0" t="n">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="124" spans="1:4">
+      <x:c r="A124" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B124" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C124" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D124" s="0" t="n">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="125" spans="1:4">
+      <x:c r="A125" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B125" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C125" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D125" s="0" t="n">
+        <x:v>72</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="126" spans="1:4">
+      <x:c r="A126" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B126" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C126" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D126" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="127" spans="1:4">
+      <x:c r="A127" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B127" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="C127" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D127" s="0" t="n">
+        <x:v>43</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="128" spans="1:4">
+      <x:c r="A128" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B128" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="C128" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D128" s="0" t="n">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="129" spans="1:4">
+      <x:c r="A129" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B129" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="C129" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D129" s="0" t="n">
+        <x:v>14.000000000000002</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="130" spans="1:4">
+      <x:c r="A130" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B130" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="C130" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D130" s="0" t="n">
+        <x:v>47</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="131" spans="1:4">
+      <x:c r="A131" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B131" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C131" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D131" s="0" t="n">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="132" spans="1:4">
+      <x:c r="A132" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B132" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C132" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D132" s="0" t="n">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="133" spans="1:4">
+      <x:c r="A133" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B133" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="C133" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D133" s="0" t="n">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="134" spans="1:4">
+      <x:c r="A134" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B134" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="C134" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D134" s="0" t="n">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="135" spans="1:4">
+      <x:c r="A135" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B135" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C135" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D135" s="0" t="n">
+        <x:v>57.99999999999999</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="136" spans="1:4">
+      <x:c r="A136" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B136" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C136" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D136" s="0" t="n">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="137" spans="1:4">
+      <x:c r="A137" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B137" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="C137" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D137" s="0" t="n">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="C98" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D98" s="0" t="s">
-        <x:v>11</x:v>
+    </x:row>
+    <x:row r="138" spans="1:4">
+      <x:c r="A138" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B138" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="C138" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D138" s="0" t="n">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="139" spans="1:4">
+      <x:c r="A139" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B139" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="C139" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D139" s="0" t="n">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="140" spans="1:4">
+      <x:c r="A140" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B140" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="C140" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D140" s="0" t="n">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="141" spans="1:4">
+      <x:c r="A141" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B141" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="C141" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D141" s="0" t="n">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="142" spans="1:4">
+      <x:c r="A142" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B142" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="C142" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D142" s="0" t="n">
+        <x:v>56.00000000000001</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="143" spans="1:4">
+      <x:c r="A143" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B143" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="C143" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D143" s="0" t="n">
+        <x:v>43</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="144" spans="1:4">
+      <x:c r="A144" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B144" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="C144" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D144" s="0" t="n">
+        <x:v>46</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="145" spans="1:4">
+      <x:c r="A145" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B145" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="C145" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D145" s="0" t="n">
+        <x:v>61</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="146" spans="1:4">
+      <x:c r="A146" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B146" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="C146" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D146" s="0" t="n">
+        <x:v>56.00000000000001</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="147" spans="1:4">
+      <x:c r="A147" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B147" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="C147" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D147" s="0" t="n">
+        <x:v>72</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="148" spans="1:4">
+      <x:c r="A148" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B148" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="C148" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D148" s="0" t="n">
+        <x:v>81</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="149" spans="1:4">
+      <x:c r="A149" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B149" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="C149" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D149" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="150" spans="1:4">
+      <x:c r="A150" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B150" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="C150" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D150" s="0" t="n">
+        <x:v>52</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="151" spans="1:4">
+      <x:c r="A151" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B151" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="C151" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D151" s="0" t="n">
+        <x:v>68</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="152" spans="1:4">
+      <x:c r="A152" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B152" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="C152" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D152" s="0" t="n">
+        <x:v>72</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="153" spans="1:4">
+      <x:c r="A153" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B153" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="C153" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D153" s="0" t="n">
+        <x:v>67</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="154" spans="1:4">
+      <x:c r="A154" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B154" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="C154" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D154" s="0" t="n">
+        <x:v>69</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="155" spans="1:4">
+      <x:c r="A155" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B155" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="C155" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D155" s="0" t="n">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="156" spans="1:4">
+      <x:c r="A156" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B156" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="C156" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D156" s="0" t="n">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="157" spans="1:4">
+      <x:c r="A157" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B157" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="C157" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D157" s="0" t="n">
+        <x:v>57.99999999999999</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="158" spans="1:4">
+      <x:c r="A158" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B158" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="C158" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D158" s="0" t="n">
+        <x:v>72</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="159" spans="1:4">
+      <x:c r="A159" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B159" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="C159" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D159" s="0" t="n">
+        <x:v>56.00000000000001</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="160" spans="1:4">
+      <x:c r="A160" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B160" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="C160" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D160" s="0" t="n">
+        <x:v>55.00000000000001</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="161" spans="1:4">
+      <x:c r="A161" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B161" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="C161" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D161" s="0" t="n">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="162" spans="1:4">
+      <x:c r="A162" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B162" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="C162" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D162" s="0" t="n">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="163" spans="1:4">
+      <x:c r="A163" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B163" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="C163" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D163" s="0" t="n">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="164" spans="1:4">
+      <x:c r="A164" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B164" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="C164" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D164" s="0" t="n">
+        <x:v>14.000000000000002</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="165" spans="1:4">
+      <x:c r="A165" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B165" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="C165" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D165" s="0" t="n">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="166" spans="1:4">
+      <x:c r="A166" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B166" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="C166" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D166" s="0" t="n">
+        <x:v>57.99999999999999</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="167" spans="1:4">
+      <x:c r="A167" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="B167" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C167" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D167" s="0" t="s">
+        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>